<commit_message>
Cleaning up print spam, added artist note, cleaned up latf (no formating yet)
</commit_message>
<xml_diff>
--- a/CCAT/bin/latf.xlsx
+++ b/CCAT/bin/latf.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Type:</t>
   </si>
@@ -73,12 +73,6 @@
   </si>
   <si>
     <t>RTP?</t>
-  </si>
-  <si>
-    <t>latest State of File:</t>
-  </si>
-  <si>
-    <t>M/Asset</t>
   </si>
 </sst>
 </file>
@@ -108,7 +102,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -147,7 +141,16 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -160,71 +163,6 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -242,78 +180,6 @@
         <color indexed="64"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -367,22 +233,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -392,28 +249,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -717,10 +568,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:N37"/>
+  <dimension ref="B1:N7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -740,363 +591,85 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H1" s="7"/>
+      <c r="H1" s="2"/>
     </row>
     <row r="2" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="F2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" s="24" t="s">
+      <c r="I2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="25" t="s">
+      <c r="J2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="25" t="s">
+      <c r="K2" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="L2" s="25" t="s">
+      <c r="L2" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="M2" s="25" t="s">
+      <c r="M2" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="N2" s="26" t="s">
+      <c r="N2" s="14" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="2"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="7"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="9"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="4"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="H4" s="7"/>
+      <c r="H4" s="2"/>
     </row>
     <row r="6" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="16" t="s">
+      <c r="F7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="15" t="s">
+      <c r="G7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="17" t="s">
+      <c r="H7" s="8" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="13"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="13"/>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="3"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="3"/>
-    </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B10" s="3"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="3"/>
-    </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B11" s="3"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="3"/>
-    </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B12" s="3"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="3"/>
-    </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B13" s="3"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="3"/>
-    </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B14" s="3"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="3"/>
-    </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B15" s="3"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="3"/>
-    </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B16" s="3"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="3"/>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="3"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="3"/>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="3"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="3"/>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="3"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="3"/>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="3"/>
-      <c r="C20" s="22"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="3"/>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="3"/>
-      <c r="C21" s="22"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="3"/>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="3"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="3"/>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="3"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="3"/>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="3"/>
-      <c r="C24" s="22"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="3"/>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="3"/>
-      <c r="C25" s="22"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="3"/>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="3"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="3"/>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="3"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="3"/>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="3"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="3"/>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B29" s="3"/>
-      <c r="C29" s="22"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="3"/>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="3"/>
-      <c r="C30" s="22"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="3"/>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="3"/>
-      <c r="C31" s="22"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="11"/>
-      <c r="H31" s="3"/>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B32" s="3"/>
-      <c r="C32" s="22"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="11"/>
-      <c r="H32" s="3"/>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B33" s="3"/>
-      <c r="C33" s="22"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="3"/>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B34" s="3"/>
-      <c r="C34" s="22"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="11"/>
-      <c r="H34" s="3"/>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B35" s="3"/>
-      <c r="C35" s="22"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="11"/>
-      <c r="H35" s="3"/>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="3"/>
-      <c r="C36" s="22"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="3"/>
-      <c r="G36" s="11"/>
-      <c r="H36" s="3"/>
-    </row>
-    <row r="37" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="1"/>
-      <c r="C37" s="23"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="5"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="12"/>
-      <c r="H37" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>